<commit_message>
updated reference section in spreadsheet
</commit_message>
<xml_diff>
--- a/documentation/List of dashboard indicators and importance language.xlsx
+++ b/documentation/List of dashboard indicators and importance language.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amoli\OneDrive\Documents\GitHub\ncw_dashboards\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E442361-F192-4DD7-82F6-78A068B7DE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4E9296-6A05-4A28-9FA9-9778ADFE9A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List of indicators" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="139">
   <si>
     <t>Diabetes</t>
   </si>
@@ -308,9 +308,6 @@
     <t>Demographics available?</t>
   </si>
   <si>
-    <t>Some/check</t>
-  </si>
-  <si>
     <t>How often data updated</t>
   </si>
   <si>
@@ -320,9 +317,6 @@
     <t xml:space="preserve">State and Individual Counties </t>
   </si>
   <si>
-    <t xml:space="preserve"> Behavioral Risk Factor Surveillance System (BRFSS) 2012-2021. Washington State Department of Health; Center for Health Statistics; Community Health Assessment Tool (CHAT); October 2023.</t>
-  </si>
-  <si>
     <t>Age-adjusted prevalence</t>
   </si>
   <si>
@@ -338,9 +332,6 @@
     <t>Age-adjusted rate per 100k</t>
   </si>
   <si>
-    <t>Washington State Department of Health, Center for Health Statistics, Death Certificate Data, 1990-2022, Community Health Assessment Tool (CHAT), November 2023.</t>
-  </si>
-  <si>
     <t>State, Individual Counties, and NCW combined</t>
   </si>
   <si>
@@ -350,33 +341,21 @@
     <t>Age, gender</t>
   </si>
   <si>
-    <t>WA Hospital Discharge Data, Comprehensive Hospitalization Abstract Reporting System (CHARS) 1987-2021. Washington State Department of Health, Center for Health Statistics, Community Health Assessment Tool (CHAT), Feb 2023. OR State Hospital Discharge Data 1987-1999. Office for Oregon Health Policy and Research. Oregon State Inpatient Database (SID) 2000-2018. Healthcare Cost and Utilization Project (HCUP), Agency for Healthcare Research and Quality. Community Health Assessment Tool (CHAT), March 2020.</t>
-  </si>
-  <si>
     <t>Age, gender (age technically possible, but we restric to age 15-19 for as close to teenage pregnancy as possible)</t>
   </si>
   <si>
-    <t>Washington State Department of Health, Center for Health Statistics, Abortion Reporting System-Report of Induced Termination of Pregnancy, 1990-2022, Community Health Assessment Tool (CHAT), November 2023. Pregnancy Data: Washington State Department of Health, Center for Health Statistics, Abortion Reporting System-Report of Induced Termination of Pregnancy, 1990-2022, Community Health Assessment Tool (CHAT), November 2023. Department of Health, Center for Health Statistics, Vital Statistics System-Washington State Certificate of Live Birth, 1990-2022, Community Health Assessment Tool (CHAT), September 2023. Department of Health, Center for Health Statistics, Vital Statistics System, Washington State Fetal Death Certificate, 1990-2022, Community Health Assessment Tool (CHAT), November 2023.</t>
-  </si>
-  <si>
     <t>Prevalence</t>
   </si>
   <si>
     <t>Percentage of days in one year</t>
   </si>
   <si>
-    <t>Centers for Disease Control and Prevention. National Environmental Public Health Tracking Network. Web. Accessed: INSERT DATE DATA WAS ACCESSED. www.cdc.gov/ephtracking</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
     <t>Individual Counties (no regional OR state data available)_</t>
   </si>
   <si>
-    <t>Center for Social Sector Analytics &amp; Technology (2023). [Graph representation of Washington state child welfare data DATE DATA ACCESSED]. Investigations &amp; Assessments (Rate). Retrieved from https://viz.portal.cssat.org/graphs/ia-rates.</t>
-  </si>
-  <si>
     <t>Rate per 1,000 housholds</t>
   </si>
   <si>
@@ -386,35 +365,711 @@
     <t>Every 2 years</t>
   </si>
   <si>
-    <t xml:space="preserve">Healthy Youth Survey. Washington State Department of Health. Accessed [DATE DATA ACCESSED]. https://www.askhys.net/ </t>
-  </si>
-  <si>
     <t>Percentage of 10th graders</t>
   </si>
   <si>
     <t>Gender identity, sexual orientation, race/ethnicity (in HYS dashboard)</t>
   </si>
   <si>
-    <t xml:space="preserve">PLACES. Centers for Disease Control and Prevention. Accessed [DATE DATA ACCESSED]. https://www.cdc.gov/places </t>
-  </si>
-  <si>
     <t xml:space="preserve">persons experiencing homelessness per 10,000 population (sheltered and unsheltered) </t>
   </si>
   <si>
     <t>Persons per 10k</t>
   </si>
   <si>
-    <t xml:space="preserve">Washington State Department of Commerce Annual Point in Time Count. Accessed [DATE DATA ACCESSED]. https://www.commerce.wa.gov/serving-communities/homelessness/annual-point-time-count/ </t>
-  </si>
-  <si>
     <t xml:space="preserve">What did we decide? </t>
+  </si>
+  <si>
+    <t>2022/2023</t>
+  </si>
+  <si>
+    <t>Percentage of infants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of kindergarteners </t>
+  </si>
+  <si>
+    <t>Yearly (goes by fiscal year)</t>
+  </si>
+  <si>
+    <t>None (there is "demographic" information, but it is not meaningful, see notes in data download instructions)</t>
+  </si>
+  <si>
+    <t>Practicing dentists per 100k</t>
+  </si>
+  <si>
+    <t>Practicing physicians per 100k</t>
+  </si>
+  <si>
+    <t>2021/2022</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Behavioral Risk Factor Surveillance System (BRFSS) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Washington State Department of Health; Center for Health Statistics; Community Health Assessment Tool (CHAT); </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATE OF DATA FROM DOWNLOAD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Behavioral Risk Factor Surveillance System (BRFSS) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Washington State Department of Health; Center for Health Statistics; Community Health Assessment Tool (CHAT); </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATE OF DATA FROM DOWNLOAD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Washington State Department of Health, Center for Health Statistics, Death Certificate Data, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Community Health Assessment Tool (CHAT), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATE OF DATA FROM DOWNLOAD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">WA Hospital Discharge Data, Comprehensive Hospitalization Abstract Reporting System (CHARS) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Washington State Department of Health, Center for Health Statistics, Community Health Assessment Tool (CHAT), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATE OF DATA FROM DOWNLOAD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. OR State Hospital Discharge Data </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Office for Oregon Health Policy and Research. Oregon State Inpatient Database (SID) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Healthcare Cost and Utilization Project (HCUP), Agency for Healthcare Research and Quality. Community Health Assessment Tool (CHAT), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATE OF DATA FROM DOWNLOAD.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Washington State Department of Health, Center for Health Statistics, Abortion Reporting System-Report of Induced Termination of Pregnancy, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Community Health Assessment Tool (CHAT), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATE OF DATA FROM DOWNLOAD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Pregnancy Data: Washington State Department of Health, Center for Health Statistics, Abortion Reporting System-Report of Induced Termination of Pregnancy, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Community Health Assessment Tool (CHAT), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATE OF DATA FROM DOWNLOAD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Department of Health, Center for Health Statistics, Vital Statistics System-Washington State Certificate of Live Birth, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Community Health Assessment Tool (CHAT), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATE OF DATA FROM DOWNLOAD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Department of Health, Center for Health Statistics, Vital Statistics System, Washington State Fetal Death Certificate, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Community Health Assessment Tool (CHAT), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATE OF DATA FROM DOWNLOAD.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> Behavioral Risk Factor Surveillance System (BRFSS) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Washington State Department of Health; Center for Health Statistics; Community Health Assessment Tool (CHAT); </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATE OF DATA FROM DOWNLOAD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>The reference for CHAT data are included directly in the data download spreadsheet, refer to that for dates</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Centers for Disease Control and Prevention. National Environmental Public Health Tracking Network. Web. Accessed: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATE DATA WAS ACCESSED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. www.cdc.gov/ephtracking</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Center for Social Sector Analytics &amp; Technology (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>APPLICABLE YEAR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">). [Graph representation of Washington state child welfare data </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DATE DATA ACCESSED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]. Investigations &amp; Assessments (Rate). Retrieved from https://viz.portal.cssat.org/graphs/ia-rates.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Healthy Youth Survey. Washington State Department of Health. Accessed [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DATE DATA ACCESSED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">]. https://www.askhys.net/ </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PLACES. Centers for Disease Control and Prevention. Accessed [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DATE DATA ACCESSED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">]. https://www.cdc.gov/places </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Washington State Department of Commerce Annual Point in Time Count. Accessed [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DATE DATA ACCESSED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">]. https://www.commerce.wa.gov/serving-communities/homelessness/annual-point-time-count/ </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Washington State Department of Health (WADOH). Washington Tracking Network (WTN). Immunization Data, County HEDIS Measures Dashboard. Web. Accessed: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATE DATA WAS ACCESSED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. https://doh.wa.gov/data-statistical-reports/washington-tracking-network-wtn/immunization-data/county-hedis-measures-dashboard </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Washington State Department of Health (WADOH). Washington Tracking Network (WTN). Immunization Data, School Immunization Data Dashboard. Web. Accessed: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATE DATA WAS ACCESSED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. https://doh.wa.gov/data-and-statistical-reports/washington-tracking-network-wtn/school-immunization/dashboard </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Health Resources &amp; Services Administration. Health Workforce: Area Health Resources Files. Web. Accessed: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATE DATA WAS ACCESSED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. https://data.hrsa.gov/topics/health-workforce/ahrf </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -445,6 +1100,29 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -486,7 +1164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -528,6 +1206,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -746,10 +1433,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J999"/>
+  <dimension ref="A1:K999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="98" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="H8" zoomScale="97" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -764,9 +1451,10 @@
     <col min="8" max="8" width="26.36328125" customWidth="1"/>
     <col min="9" max="9" width="102" customWidth="1"/>
     <col min="10" max="10" width="61.453125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="31.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -774,10 +1462,10 @@
         <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>88</v>
@@ -797,8 +1485,11 @@
       <c r="J1" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="K1" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="51.5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -809,28 +1500,31 @@
         <v>2021</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="F2" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>36</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="J2" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="51.5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -841,28 +1535,31 @@
         <v>2021</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="F3" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>38</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="J3" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="51.5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -873,28 +1570,31 @@
         <v>2021</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="F4" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>40</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="12" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="J4" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="12" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>42</v>
       </c>
@@ -903,12 +1603,10 @@
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E5" s="8"/>
-      <c r="F5" s="9" t="s">
-        <v>91</v>
-      </c>
+      <c r="F5" s="9"/>
       <c r="G5" s="9" t="s">
         <v>3</v>
       </c>
@@ -918,7 +1616,7 @@
       </c>
       <c r="J5" s="11"/>
     </row>
-    <row r="6" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="38.5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -929,28 +1627,31 @@
         <v>2022</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>44</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="J6" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="38.5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -961,28 +1662,31 @@
         <v>2022</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="J7" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="50" x14ac:dyDescent="0.25">
+      <c r="J7" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="K7" s="20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="50.5" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -993,28 +1697,31 @@
         <v>2022</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>48</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="J8" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="60.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="60.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1025,28 +1732,31 @@
         <v>2022</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>50</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="J9" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="104" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="K9" s="20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="122" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1057,28 +1767,31 @@
         <v>2021</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>52</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="J10" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+      <c r="J10" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="K10" s="20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="180" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1089,13 +1802,13 @@
         <v>2022</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>102</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>106</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>54</v>
@@ -1104,11 +1817,14 @@
       <c r="I11" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="J11" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="17" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="J11" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="17" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>10</v>
       </c>
@@ -1117,7 +1833,7 @@
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="14"/>
@@ -1125,14 +1841,14 @@
         <v>11</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="I12" s="15" t="s">
         <v>57</v>
       </c>
       <c r="J12" s="16"/>
     </row>
-    <row r="13" spans="1:10" s="17" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="17" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>12</v>
       </c>
@@ -1141,7 +1857,7 @@
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="14"/>
@@ -1149,14 +1865,14 @@
         <v>13</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="I13" s="15" t="s">
         <v>58</v>
       </c>
       <c r="J13" s="16"/>
     </row>
-    <row r="14" spans="1:10" s="17" customFormat="1" ht="50" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="17" customFormat="1" ht="50" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>14</v>
       </c>
@@ -1165,7 +1881,7 @@
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="14"/>
@@ -1173,14 +1889,14 @@
         <v>59</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="I14" s="15" t="s">
         <v>60</v>
       </c>
       <c r="J14" s="16"/>
     </row>
-    <row r="15" spans="1:10" s="17" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="17" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>15</v>
       </c>
@@ -1189,7 +1905,7 @@
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="14"/>
@@ -1197,14 +1913,14 @@
         <v>16</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="I15" s="15" t="s">
         <v>61</v>
       </c>
       <c r="J15" s="16"/>
     </row>
-    <row r="16" spans="1:10" ht="46" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="46" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
@@ -1215,28 +1931,28 @@
         <v>2019</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="J16" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="50" x14ac:dyDescent="0.25">
+      <c r="J16" s="20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="51.5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>64</v>
       </c>
@@ -1247,28 +1963,28 @@
         <v>2019</v>
       </c>
       <c r="D17" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="F17" s="7" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>66</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="J17" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="J17" s="20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="38" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>74</v>
       </c>
@@ -1279,28 +1995,28 @@
         <v>2021</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>76</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="J18" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="50" x14ac:dyDescent="0.25">
+      <c r="J18" s="20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="50.5" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>78</v>
       </c>
@@ -1311,28 +2027,28 @@
         <v>2021</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>23</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="J19" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="J19" s="20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="38" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>24</v>
       </c>
@@ -1343,28 +2059,28 @@
         <v>2021</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>25</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="J20" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="50" x14ac:dyDescent="0.25">
+      <c r="J20" s="20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="50.5" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>26</v>
       </c>
@@ -1375,28 +2091,28 @@
         <v>2023</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>82</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="J21" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="50" x14ac:dyDescent="0.25">
+      <c r="J21" s="20" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="50.5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>19</v>
       </c>
@@ -1407,101 +2123,153 @@
         <v>2023</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="J22" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="J22" s="20" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="7"/>
+      <c r="C23" s="19">
+        <v>2021</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>105</v>
+      </c>
       <c r="G23" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H23" s="5"/>
+      <c r="H23" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="I23" s="6" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="J23" s="20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="7"/>
+      <c r="C24" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>105</v>
+      </c>
       <c r="G24" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="5"/>
+      <c r="H24" s="5" t="s">
+        <v>117</v>
+      </c>
       <c r="I24" s="6" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="J24" s="20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="50.5" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>70</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="7"/>
+      <c r="C25" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>119</v>
+      </c>
       <c r="G25" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H25" s="5"/>
+      <c r="H25" s="5" t="s">
+        <v>120</v>
+      </c>
       <c r="I25" s="6" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="J25" s="20" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="50.5" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="7"/>
+      <c r="C26" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>119</v>
+      </c>
       <c r="G26" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H26" s="5"/>
+      <c r="H26" s="5" t="s">
+        <v>121</v>
+      </c>
       <c r="I26" s="6" t="s">
         <v>73</v>
+      </c>
+      <c r="J26" s="20" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>